<commit_message>
Missed component in VR BOM
</commit_message>
<xml_diff>
--- a/reference/hardware/VR Conditioner/VR_bom.xlsx
+++ b/reference/hardware/VR Conditioner/VR_bom.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="72">
   <si>
     <t>Value</t>
   </si>
@@ -228,6 +228,21 @@
   </si>
   <si>
     <t>Digikey import</t>
+  </si>
+  <si>
+    <t>R10,R12</t>
+  </si>
+  <si>
+    <t>4.3k</t>
+  </si>
+  <si>
+    <t>RES 4.7K OHM 2W 5% AXIAL</t>
+  </si>
+  <si>
+    <t>FMP200JR-52-4K7</t>
+  </si>
+  <si>
+    <t>4.7KZCT-ND</t>
   </si>
 </sst>
 </file>
@@ -868,10 +883,10 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:S14"/>
+  <dimension ref="A1:S15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="99" workbookViewId="0">
-      <selection activeCell="S21" sqref="S21"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="99" workbookViewId="0">
+      <selection activeCell="Q6" sqref="Q6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -966,7 +981,7 @@
       <c r="O2" s="3"/>
       <c r="P2" s="4"/>
       <c r="Q2" s="4" t="str">
-        <f>IF(NOT(J2=""),A2&amp;","&amp;J2,"")</f>
+        <f t="shared" ref="Q2:Q14" si="0">IF(NOT(J2=""),A2&amp;","&amp;J2,"")</f>
         <v/>
       </c>
       <c r="R2" t="str">
@@ -1010,16 +1025,16 @@
         <v>0</v>
       </c>
       <c r="N3" s="6">
-        <f>L3*A3</f>
+        <f t="shared" ref="N3:N9" si="1">L3*A3</f>
         <v>0.2</v>
       </c>
       <c r="O3" s="6">
-        <f>M3*A3</f>
+        <f t="shared" ref="O3:O9" si="2">M3*A3</f>
         <v>0</v>
       </c>
       <c r="P3" s="4"/>
       <c r="Q3" s="4" t="str">
-        <f>IF(NOT(J3=""),A3&amp;","&amp;J3,"")</f>
+        <f t="shared" si="0"/>
         <v>2,311-1.00KCRCT-ND</v>
       </c>
       <c r="R3" t="str">
@@ -1027,7 +1042,7 @@
         <v>Resistor - 2x 1k</v>
       </c>
       <c r="S3" t="str">
-        <f>IF(NOT(K3=""),K3&amp;"|"&amp;A3,"")</f>
+        <f t="shared" ref="S3:S14" si="3">IF(NOT(K3=""),K3&amp;"|"&amp;A3,"")</f>
         <v/>
       </c>
     </row>
@@ -1076,7 +1091,7 @@
       </c>
       <c r="P4" s="4"/>
       <c r="Q4" s="4" t="str">
-        <f>IF(NOT(J4=""),A4&amp;","&amp;J4,"")</f>
+        <f t="shared" si="0"/>
         <v>6,311-10KARCT-ND</v>
       </c>
       <c r="R4" t="str">
@@ -1084,23 +1099,23 @@
         <v>Resistor - 6x 10k</v>
       </c>
       <c r="S4" t="str">
-        <f>IF(NOT(K4=""),K4&amp;"|"&amp;A4,"")</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="5" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="14">
         <f>LEN(B5)-LEN(SUBSTITUTE(B5,",",""))+1</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>28</v>
+        <v>67</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>43</v>
+        <v>68</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>69</v>
       </c>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
@@ -1111,21 +1126,19 @@
         <v>18</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>41</v>
+        <v>70</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>42</v>
+        <v>71</v>
       </c>
       <c r="K5" s="2"/>
       <c r="L5" s="5">
-        <v>0.1</v>
-      </c>
-      <c r="M5" s="5">
-        <v>0</v>
-      </c>
+        <v>0.2</v>
+      </c>
+      <c r="M5" s="5"/>
       <c r="N5" s="6">
         <f>L5*A5</f>
-        <v>0.1</v>
+        <v>0.4</v>
       </c>
       <c r="O5" s="6">
         <f>M5*A5</f>
@@ -1133,15 +1146,15 @@
       </c>
       <c r="P5" s="4"/>
       <c r="Q5" s="4" t="str">
-        <f>IF(NOT(J5=""),A5&amp;","&amp;J5,"")</f>
-        <v>1,311-1136-1-ND</v>
+        <f t="shared" ref="Q5" si="4">IF(NOT(J5=""),A5&amp;","&amp;J5,"")</f>
+        <v>2,4.7KZCT-ND</v>
       </c>
       <c r="R5" t="str">
-        <f>"Capacitor - " &amp;A5&amp;"x "&amp;C5</f>
-        <v>Capacitor - 1x 0.01uF</v>
+        <f>"Resistor - " &amp;A5&amp;"x "&amp;C5</f>
+        <v>Resistor - 2x 4.3k</v>
       </c>
       <c r="S5" t="str">
-        <f>IF(NOT(K5=""),K5&amp;"|"&amp;A5,"")</f>
+        <f t="shared" ref="S5" si="5">IF(NOT(K5=""),K5&amp;"|"&amp;A5,"")</f>
         <v/>
       </c>
     </row>
@@ -1151,13 +1164,13 @@
         <v>1</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
@@ -1168,10 +1181,10 @@
         <v>18</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="K6" s="2"/>
       <c r="L6" s="5">
@@ -1181,40 +1194,40 @@
         <v>0</v>
       </c>
       <c r="N6" s="6">
-        <f>L6*A6</f>
+        <f t="shared" si="1"/>
         <v>0.1</v>
       </c>
       <c r="O6" s="6">
-        <f>M6*A6</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="P6" s="4"/>
       <c r="Q6" s="4" t="str">
-        <f>IF(NOT(J6=""),A6&amp;","&amp;J6,"")</f>
-        <v>1,311-1365-1-ND</v>
+        <f t="shared" si="0"/>
+        <v>1,311-1136-1-ND</v>
       </c>
       <c r="R6" t="str">
         <f>"Capacitor - " &amp;A6&amp;"x "&amp;C6</f>
-        <v>Capacitor - 1x 1uF</v>
+        <v>Capacitor - 1x 0.01uF</v>
       </c>
       <c r="S6" t="str">
-        <f>IF(NOT(K6=""),K6&amp;"|"&amp;A6,"")</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="7" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="14">
-        <f t="shared" ref="A7:A8" si="0">LEN(B7)-LEN(SUBSTITUTE(B7,",",""))+1</f>
-        <v>2</v>
+        <f>LEN(B7)-LEN(SUBSTITUTE(B7,",",""))+1</f>
+        <v>1</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>49</v>
+        <v>8</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>45</v>
       </c>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
@@ -1225,10 +1238,10 @@
         <v>18</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="K7" s="2"/>
       <c r="L7" s="5">
@@ -1238,40 +1251,40 @@
         <v>0</v>
       </c>
       <c r="N7" s="6">
-        <f>L7*A7</f>
-        <v>0.2</v>
+        <f t="shared" si="1"/>
+        <v>0.1</v>
       </c>
       <c r="O7" s="6">
-        <f>M7*A7</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="P7" s="4"/>
       <c r="Q7" s="4" t="str">
-        <f>IF(NOT(J7=""),A7&amp;","&amp;J7,"")</f>
-        <v>2,311-1127-1-ND</v>
+        <f t="shared" si="0"/>
+        <v>1,311-1365-1-ND</v>
       </c>
       <c r="R7" t="str">
         <f>"Capacitor - " &amp;A7&amp;"x "&amp;C7</f>
-        <v>Capacitor - 2x 1nF</v>
+        <v>Capacitor - 1x 1uF</v>
       </c>
       <c r="S7" t="str">
-        <f>IF(NOT(K7=""),K7&amp;"|"&amp;A7,"")</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="8" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="14">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <f t="shared" ref="A8:A9" si="6">LEN(B8)-LEN(SUBSTITUTE(B8,",",""))+1</f>
+        <v>2</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
@@ -1282,10 +1295,10 @@
         <v>18</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="K8" s="2"/>
       <c r="L8" s="5">
@@ -1295,50 +1308,81 @@
         <v>0</v>
       </c>
       <c r="N8" s="6">
-        <f>L8*A8</f>
-        <v>0.1</v>
+        <f t="shared" si="1"/>
+        <v>0.2</v>
       </c>
       <c r="O8" s="6">
-        <f>M8*A8</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="P8" s="4"/>
       <c r="Q8" s="4" t="str">
-        <f>IF(NOT(J8=""),A8&amp;","&amp;J8,"")</f>
-        <v>1,311-1361-1-ND</v>
+        <f t="shared" si="0"/>
+        <v>2,311-1127-1-ND</v>
       </c>
       <c r="R8" t="str">
         <f>"Capacitor - " &amp;A8&amp;"x "&amp;C8</f>
-        <v>Capacitor - 1x 0.1uF</v>
+        <v>Capacitor - 2x 1nF</v>
       </c>
       <c r="S8" t="str">
-        <f>IF(NOT(K8=""),K8&amp;"|"&amp;A8,"")</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="9" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="12"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
+      <c r="A9" s="14">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>57</v>
+      </c>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
-      <c r="J9" s="2"/>
+      <c r="G9" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>56</v>
+      </c>
       <c r="K9" s="2"/>
-      <c r="L9" s="3"/>
-      <c r="M9" s="3"/>
-      <c r="N9" s="3"/>
-      <c r="O9" s="6"/>
+      <c r="L9" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="M9" s="5">
+        <v>0</v>
+      </c>
+      <c r="N9" s="6">
+        <f t="shared" si="1"/>
+        <v>0.1</v>
+      </c>
+      <c r="O9" s="6">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="P9" s="4"/>
       <c r="Q9" s="4" t="str">
-        <f>IF(NOT(J9=""),A9&amp;","&amp;J9,"")</f>
-        <v/>
+        <f t="shared" si="0"/>
+        <v>1,311-1361-1-ND</v>
+      </c>
+      <c r="R9" t="str">
+        <f>"Capacitor - " &amp;A9&amp;"x "&amp;C9</f>
+        <v>Capacitor - 1x 0.1uF</v>
       </c>
       <c r="S9" t="str">
-        <f>IF(NOT(K9=""),K9&amp;"|"&amp;A9,"")</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
@@ -1360,111 +1404,78 @@
       <c r="O10" s="6"/>
       <c r="P10" s="4"/>
       <c r="Q10" s="4" t="str">
-        <f>IF(NOT(J10=""),A10&amp;","&amp;J10,"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="S10" t="str">
-        <f>IF(NOT(K10=""),K10&amp;"|"&amp;A10,"")</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="11" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="14">
-        <f>LEN(B11)-LEN(SUBSTITUTE(B11,",",""))+1</f>
-        <v>1</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>50</v>
-      </c>
+      <c r="A11" s="12"/>
+      <c r="B11" s="4"/>
       <c r="C11" s="3"/>
-      <c r="D11" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>54</v>
-      </c>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
       <c r="F11" s="3"/>
-      <c r="G11" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="H11" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="I11" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="J11" s="2" t="s">
-        <v>51</v>
-      </c>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="2"/>
       <c r="K11" s="2"/>
-      <c r="L11" s="5">
-        <v>7.19</v>
-      </c>
-      <c r="M11" s="5">
-        <v>0</v>
-      </c>
-      <c r="N11" s="6">
-        <f>L11*A11</f>
-        <v>7.19</v>
-      </c>
-      <c r="O11" s="6">
-        <f>M11*A11</f>
-        <v>0</v>
-      </c>
+      <c r="L11" s="3"/>
+      <c r="M11" s="3"/>
+      <c r="N11" s="3"/>
+      <c r="O11" s="6"/>
       <c r="P11" s="4"/>
       <c r="Q11" s="4" t="str">
-        <f>IF(NOT(J11=""),A11&amp;","&amp;J11,"")</f>
-        <v>1,MAX9926UAEE+TCT-ND</v>
-      </c>
-      <c r="R11" t="str">
-        <f>"IC- " &amp;A11&amp;"x "&amp;C11</f>
-        <v xml:space="preserve">IC- 1x </v>
+        <f t="shared" si="0"/>
+        <v/>
       </c>
       <c r="S11" t="str">
-        <f>IF(NOT(K11=""),K11&amp;"|"&amp;A11,"")</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:19" ht="27" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="14">
         <f>LEN(B12)-LEN(SUBSTITUTE(B12,",",""))+1</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>61</v>
+        <v>50</v>
+      </c>
+      <c r="C12" s="3"/>
+      <c r="D12" s="7" t="s">
+        <v>65</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="F12" s="3"/>
       <c r="G12" s="3" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="H12" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I12" s="3" t="s">
-        <v>62</v>
+      <c r="I12" s="7" t="s">
+        <v>52</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="K12" s="2"/>
       <c r="L12" s="5">
-        <v>0.14000000000000001</v>
+        <v>7.19</v>
       </c>
       <c r="M12" s="5">
         <v>0</v>
       </c>
       <c r="N12" s="6">
         <f>L12*A12</f>
-        <v>0.28000000000000003</v>
+        <v>7.19</v>
       </c>
       <c r="O12" s="6">
         <f>M12*A12</f>
@@ -1472,42 +1483,58 @@
       </c>
       <c r="P12" s="4"/>
       <c r="Q12" s="4" t="str">
-        <f>IF(NOT(J12=""),A12&amp;","&amp;J12,"")</f>
-        <v xml:space="preserve">2,952-2265-ND </v>
+        <f t="shared" si="0"/>
+        <v>1,MAX9926UAEE+TCT-ND</v>
       </c>
       <c r="R12" t="str">
-        <f>"Pins- " &amp;A12&amp;"x "&amp;C12</f>
-        <v>Pins- 2x 0.100"</v>
+        <f>"IC- " &amp;A12&amp;"x "&amp;C12</f>
+        <v xml:space="preserve">IC- 1x </v>
       </c>
       <c r="S12" t="str">
-        <f>IF(NOT(K12=""),K12&amp;"|"&amp;A12,"")</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" ht="27" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="14">
         <f>LEN(B13)-LEN(SUBSTITUTE(B13,",",""))+1</f>
-        <v>1</v>
-      </c>
-      <c r="B13" s="4"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
+        <v>2</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>60</v>
+      </c>
       <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
-      <c r="I13" s="3"/>
-      <c r="J13" s="2"/>
+      <c r="G13" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I13" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>58</v>
+      </c>
       <c r="K13" s="2"/>
       <c r="L13" s="5">
-        <v>0</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="M13" s="5">
         <v>0</v>
       </c>
       <c r="N13" s="6">
         <f>L13*A13</f>
-        <v>0</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="O13" s="6">
         <f>M13*A13</f>
@@ -1515,47 +1542,90 @@
       </c>
       <c r="P13" s="4"/>
       <c r="Q13" s="4" t="str">
-        <f>IF(NOT(J13=""),A13&amp;","&amp;J13,"")</f>
-        <v/>
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">2,952-2265-ND </v>
+      </c>
+      <c r="R13" t="str">
+        <f>"Pins- " &amp;A13&amp;"x "&amp;C13</f>
+        <v>Pins- 2x 0.100"</v>
       </c>
       <c r="S13" t="str">
-        <f>IF(NOT(K13=""),K13&amp;"|"&amp;A13,"")</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="14" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="12"/>
+      <c r="A14" s="14">
+        <f>LEN(B14)-LEN(SUBSTITUTE(B14,",",""))+1</f>
+        <v>1</v>
+      </c>
       <c r="B14" s="4"/>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
-      <c r="F14" s="16"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="8"/>
-      <c r="I14" s="18" t="s">
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
+      <c r="L14" s="5">
+        <v>0</v>
+      </c>
+      <c r="M14" s="5">
+        <v>0</v>
+      </c>
+      <c r="N14" s="6">
+        <f>L14*A14</f>
+        <v>0</v>
+      </c>
+      <c r="O14" s="6">
+        <f>M14*A14</f>
+        <v>0</v>
+      </c>
+      <c r="P14" s="4"/>
+      <c r="Q14" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="S14" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="15" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="12"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="16"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="8"/>
+      <c r="I15" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="J14" s="19"/>
-      <c r="K14" s="17"/>
-      <c r="L14" s="1" t="s">
+      <c r="J15" s="19"/>
+      <c r="K15" s="17"/>
+      <c r="L15" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="M14" s="1"/>
-      <c r="N14" s="10">
-        <f>SUM(N2:N13)</f>
-        <v>8.77</v>
-      </c>
-      <c r="O14" s="10">
-        <f>SUM(O2:O13)</f>
-        <v>0</v>
-      </c>
-      <c r="P14" s="9" t="s">
+      <c r="M15" s="1"/>
+      <c r="N15" s="10">
+        <f>SUM(N2:N14)</f>
+        <v>9.17</v>
+      </c>
+      <c r="O15" s="10">
+        <f>SUM(O2:O14)</f>
+        <v>0</v>
+      </c>
+      <c r="P15" s="9" t="s">
         <v>13</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="I14:J14"/>
+    <mergeCell ref="I15:J15"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.75000000000000011" right="0.75000000000000011" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>